<commit_message>
Revert "Merge branch 'main' into waowaowiwaow"
This reverts commit 34cab4aacb1ecba34356d512a313464dd206435a, reversing
changes made to 1914f5844a7c93437d4586b966ad3d62ce6413d4.
</commit_message>
<xml_diff>
--- a/xlsx/sample.xlsx
+++ b/xlsx/sample.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">DIGITAL</t>
   </si>
   <si>
-    <t xml:space="preserve">Vinoya</t>
+    <t xml:space="preserve">Vinoya </t>
   </si>
   <si>
     <t xml:space="preserve">Cedrick Anne </t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">cedrickannavinoya03@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Ann Michel Pascual</t>
+    <t xml:space="preserve">Ann Michel Pascual </t>
   </si>
   <si>
     <t xml:space="preserve">Mother </t>
@@ -204,7 +204,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -266,6 +266,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <u val="single"/>
@@ -356,67 +362,67 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -674,8 +680,8 @@
   </sheetPr>
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q9" activeCellId="0" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
NAGANA NA YUNG PROGRESS BAR
</commit_message>
<xml_diff>
--- a/xlsx/sample.xlsx
+++ b/xlsx/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -178,22 +178,19 @@
     <t xml:space="preserve">REL</t>
   </si>
   <si>
-    <t xml:space="preserve">ST 7669 0924 0000 0000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Student - Plan A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angeles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenneth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ye22ah@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eddrin Desiderio</t>
+    <t xml:space="preserve">ST 7669 0924 0000 -1213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST 7669 0924 0000 -2427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST 7669 0924 0000 -3641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST 7669 0924 0000 -4855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST 7669 0924 0000 -6069</t>
   </si>
 </sst>
 </file>
@@ -204,7 +201,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -268,12 +265,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
@@ -357,73 +348,77 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -678,10 +673,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q9" activeCellId="0" sqref="Q9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -916,53 +911,255 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v>45717</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="12" t="n">
+        <v>32721</v>
+      </c>
+      <c r="J4" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="11" t="n">
+        <v>-8449817565</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="15" t="n">
-        <v>45712</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E5" s="15" t="n">
+        <v>45722</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="15" t="n">
+        <v>28550</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>-17223869364</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="C6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="12" t="n">
+        <v>45727</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="12" t="n">
+        <v>24379</v>
+      </c>
+      <c r="J6" s="11" t="n">
+        <v>48</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="11" t="n">
+        <v>-25997921163</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="C7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="15" t="n">
+        <v>45732</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="15" t="n">
+        <v>20208</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>-34771972962</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="12" t="n">
+        <v>45737</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="15" t="n">
-        <v>36892</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O4" s="14" t="s">
-        <v>51</v>
+      <c r="I8" s="12" t="n">
+        <v>16037</v>
+      </c>
+      <c r="J8" s="11" t="n">
+        <v>66</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="11" t="n">
+        <v>-43546024761</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M3" r:id="rId1" display="yeah@gmail.com"/>
-    <hyperlink ref="M4" r:id="rId2" display="ye22ah@gmail.com"/>
+    <hyperlink ref="M5" r:id="rId2" display="yeah@gmail.com"/>
+    <hyperlink ref="M7" r:id="rId3" display="yeah@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>